<commit_message>
Update Seed Germination Files
</commit_message>
<xml_diff>
--- a/BIO 221/Seed Germination/Seed Germination Data.xlsx
+++ b/BIO 221/Seed Germination/Seed Germination Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Purva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IISER\Labs\BIO 221\Seed Germination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27241295-0ED2-49EA-A86E-B01F11F1B9CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CF2761-668D-40C3-9A1D-0A5339AB9A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Number of Seeds Germinated" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t>Control</t>
   </si>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,6 +188,12 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,8 +414,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -608,78 +614,218 @@
       <c r="A7" s="6"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="6"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="6"/>
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="16">
+        <v>19</v>
+      </c>
+      <c r="C9" s="16">
+        <v>20</v>
+      </c>
+      <c r="D9" s="16">
+        <f>(B9/C9)*100</f>
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="6"/>
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="16">
+        <v>16</v>
+      </c>
+      <c r="C10" s="16">
+        <v>20</v>
+      </c>
+      <c r="D10" s="16">
+        <f>(B10/C10)*100</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="6"/>
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16">
+        <v>17</v>
+      </c>
+      <c r="C11" s="16">
+        <v>20</v>
+      </c>
+      <c r="D11" s="16">
+        <f>(B11/C11)*100</f>
+        <v>85</v>
+      </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="6"/>
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="16">
+        <v>18</v>
+      </c>
+      <c r="C12" s="16">
+        <v>20</v>
+      </c>
+      <c r="D12" s="16">
+        <f>(B12/C12)*100</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="6"/>
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="16">
+        <v>18</v>
+      </c>
+      <c r="C13" s="16">
+        <v>20</v>
+      </c>
+      <c r="D13" s="16">
+        <f>(B13/C13)*100</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="6"/>
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16">
+        <v>18</v>
+      </c>
+      <c r="C14" s="16">
+        <v>20</v>
+      </c>
+      <c r="D14" s="16">
+        <f>(B14/C14)*100</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="6"/>
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="16">
+        <v>20</v>
+      </c>
+      <c r="C15" s="16">
+        <v>20</v>
+      </c>
+      <c r="D15" s="16">
+        <f>(B15/C15)*100</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="16">
+        <v>20</v>
+      </c>
+      <c r="C16" s="16">
+        <v>20</v>
+      </c>
+      <c r="D16" s="16">
+        <f>(B16/C16)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17">
+        <v>17</v>
+      </c>
+      <c r="C17" s="17">
+        <v>17</v>
+      </c>
+      <c r="D17" s="17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="16">
+        <v>16</v>
+      </c>
+      <c r="C18" s="16">
+        <v>20</v>
+      </c>
+      <c r="D18" s="16">
+        <f>(B18/C18)*100</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="16">
+        <v>18</v>
+      </c>
+      <c r="C19" s="16">
+        <v>20</v>
+      </c>
+      <c r="D19" s="16">
+        <f>(B19/C19)*100</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:4">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:4">
       <c r="A22" s="6"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:4">
       <c r="A23" s="6"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:4">
       <c r="A24" s="6"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:4">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:4">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:4">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:4">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:4">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:4">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:4">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:4">
       <c r="A32" s="6"/>
     </row>
     <row r="33" spans="1:1">
@@ -3598,8 +3744,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>